<commit_message>
Add Google OAuth integration and authentication system
</commit_message>
<xml_diff>
--- a/Server/Data/WeeklyDeal.xlsx
+++ b/Server/Data/WeeklyDeal.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -24,6 +24,21 @@
   </si>
   <si>
     <t xml:space="preserve">Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing Second Deal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test Second Deal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ertRTGERG</t>
   </si>
 </sst>
 </file>
@@ -58,7 +73,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -68,24 +83,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.43" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="0">
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0">
+        <v>25.99</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="0">
+        <v>12.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>